<commit_message>
Mise en page du fichier excel
</commit_message>
<xml_diff>
--- a/graph/Climat.xlsx
+++ b/graph/Climat.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johann\Documents\TP1_Qualite_Donnees\graph\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bivaudb/Desktop/EPSI/QUALITE DES DONNES/TP1_Qualite_Donnees/graph/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0765AAE2-D331-4F2F-94CA-E2FE95427721}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BB22F6-F00B-CE41-A503-A1BB7FC280DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="285" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SI " sheetId="2" r:id="rId1"/>
     <sheet name="SI -erreur" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -26,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="60">
   <si>
     <t>janvier</t>
   </si>
@@ -161,9 +170,6 @@
   </si>
   <si>
     <t>écart type</t>
-  </si>
-  <si>
-    <t>Température moyenne relevée entre 8H du matin et 18H</t>
   </si>
   <si>
     <t>min /max</t>
@@ -757,13 +763,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -801,7 +807,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -842,7 +848,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -883,7 +889,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -924,7 +930,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -965,7 +971,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1006,7 +1012,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1047,7 +1053,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1088,7 +1094,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1129,7 +1135,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1170,7 +1176,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1211,7 +1217,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1252,7 +1258,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1294,7 +1300,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1335,7 +1341,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1376,7 +1382,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1417,7 +1423,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1458,7 +1464,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1499,7 +1505,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1540,7 +1546,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1581,7 +1587,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1623,7 +1629,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1664,7 +1670,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1705,7 +1711,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1746,7 +1752,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1787,7 +1793,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1828,7 +1834,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1869,7 +1875,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1910,7 +1916,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1951,7 +1957,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -1990,7 +1996,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -2029,7 +2035,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -2073,1386 +2079,1381 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="I3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="K3" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="L3" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="M3" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="N3" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="O3" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>12</v>
+      </c>
+      <c r="B3">
+        <v>-5</v>
+      </c>
+      <c r="C3">
+        <v>-7</v>
+      </c>
+      <c r="D3">
+        <v>-7</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>12</v>
+      </c>
+      <c r="G3">
+        <v>17</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>20</v>
+      </c>
+      <c r="J3">
+        <v>16</v>
+      </c>
+      <c r="K3">
+        <v>6</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>-6</v>
+      </c>
+      <c r="C4">
+        <v>-6</v>
+      </c>
+      <c r="D4">
+        <v>-8</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <v>19</v>
+      </c>
+      <c r="J4">
+        <v>14</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>-5</v>
+      </c>
+      <c r="C5">
+        <v>-5</v>
       </c>
       <c r="D5">
         <v>-5</v>
       </c>
       <c r="E5">
-        <v>-7</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>-7</v>
+        <v>15</v>
       </c>
       <c r="G5">
+        <v>17</v>
+      </c>
+      <c r="H5">
+        <v>17</v>
+      </c>
+      <c r="I5">
+        <v>19</v>
+      </c>
+      <c r="J5">
+        <v>15</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
         <v>2</v>
       </c>
-      <c r="H5">
+      <c r="M5">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>-3</v>
+      </c>
+      <c r="C6">
+        <v>-6</v>
+      </c>
+      <c r="D6">
+        <v>-3</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>16</v>
+      </c>
+      <c r="G6">
+        <v>14</v>
+      </c>
+      <c r="H6">
+        <v>18</v>
+      </c>
+      <c r="I6">
+        <v>18</v>
+      </c>
+      <c r="J6">
+        <v>13</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>-6</v>
+      </c>
+      <c r="C7">
+        <v>-8</v>
+      </c>
+      <c r="D7">
+        <v>-2</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>17</v>
+      </c>
+      <c r="I7">
+        <v>17</v>
+      </c>
+      <c r="J7">
         <v>12</v>
       </c>
-      <c r="I5">
-        <v>17</v>
-      </c>
-      <c r="J5">
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>-11</v>
+      </c>
+      <c r="C8">
+        <v>-9</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>12</v>
+      </c>
+      <c r="G8">
+        <v>17</v>
+      </c>
+      <c r="H8">
+        <v>17</v>
+      </c>
+      <c r="I8">
+        <v>18</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+      <c r="M8">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>-6</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>17</v>
+      </c>
+      <c r="H9">
+        <v>16</v>
+      </c>
+      <c r="I9">
+        <v>16</v>
+      </c>
+      <c r="J9">
+        <v>12</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9">
+        <v>4</v>
+      </c>
+      <c r="M9">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>-8</v>
+      </c>
+      <c r="C10">
+        <v>-11</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>7</v>
+      </c>
+      <c r="G10">
+        <v>15</v>
+      </c>
+      <c r="H10">
+        <v>17</v>
+      </c>
+      <c r="I10">
+        <v>17</v>
+      </c>
+      <c r="J10">
+        <v>11</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+      <c r="M10">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="K5">
-        <v>20</v>
-      </c>
-      <c r="L5">
-        <v>16</v>
-      </c>
-      <c r="M5">
+      <c r="B11">
+        <v>-11</v>
+      </c>
+      <c r="C11">
+        <v>-12</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>7</v>
+      </c>
+      <c r="F11">
         <v>6</v>
       </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6">
-        <v>-6</v>
-      </c>
-      <c r="E6">
-        <v>-6</v>
-      </c>
-      <c r="F6">
-        <v>-8</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6">
+      <c r="G11">
         <v>14</v>
       </c>
-      <c r="I6">
-        <v>16</v>
-      </c>
-      <c r="J6">
-        <v>20</v>
-      </c>
-      <c r="K6">
-        <v>19</v>
-      </c>
-      <c r="L6">
+      <c r="H11">
+        <v>17</v>
+      </c>
+      <c r="I11">
+        <v>15</v>
+      </c>
+      <c r="J11">
+        <v>11</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+      <c r="L11">
+        <v>5</v>
+      </c>
+      <c r="M11">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>-8</v>
+      </c>
+      <c r="C12">
+        <v>-9</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12">
+        <v>15</v>
+      </c>
+      <c r="I12">
         <v>14</v>
       </c>
-      <c r="M6">
-        <v>2</v>
-      </c>
-      <c r="N6">
+      <c r="J12">
+        <v>12</v>
+      </c>
+      <c r="K12">
+        <v>4</v>
+      </c>
+      <c r="L12">
+        <v>-1</v>
+      </c>
+      <c r="M12">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>-8</v>
+      </c>
+      <c r="C13">
+        <v>-6</v>
+      </c>
+      <c r="D13">
         <v>1</v>
       </c>
-      <c r="O6">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="E13">
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
         <v>14</v>
       </c>
-      <c r="D7">
-        <v>-5</v>
-      </c>
-      <c r="E7">
-        <v>-5</v>
-      </c>
-      <c r="F7">
-        <v>-5</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
-      <c r="H7">
-        <v>15</v>
-      </c>
-      <c r="I7">
-        <v>17</v>
-      </c>
-      <c r="J7">
-        <v>17</v>
-      </c>
-      <c r="K7">
-        <v>19</v>
-      </c>
-      <c r="L7">
-        <v>15</v>
-      </c>
-      <c r="M7">
-        <v>3</v>
-      </c>
-      <c r="N7">
-        <v>2</v>
-      </c>
-      <c r="O7">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8">
-        <v>-3</v>
-      </c>
-      <c r="E8">
-        <v>-6</v>
-      </c>
-      <c r="F8">
-        <v>-3</v>
-      </c>
-      <c r="G8">
-        <v>6</v>
-      </c>
-      <c r="H8">
-        <v>16</v>
-      </c>
-      <c r="I8">
-        <v>14</v>
-      </c>
-      <c r="J8">
-        <v>18</v>
-      </c>
-      <c r="K8">
-        <v>18</v>
-      </c>
-      <c r="L8">
-        <v>13</v>
-      </c>
-      <c r="M8">
-        <v>4</v>
-      </c>
-      <c r="N8">
-        <v>3</v>
-      </c>
-      <c r="O8">
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9">
-        <v>-6</v>
-      </c>
-      <c r="E9">
-        <v>-8</v>
-      </c>
-      <c r="F9">
-        <v>-2</v>
-      </c>
-      <c r="G9">
-        <v>4</v>
-      </c>
-      <c r="H9">
-        <v>13</v>
-      </c>
-      <c r="I9">
-        <v>15</v>
-      </c>
-      <c r="J9">
-        <v>17</v>
-      </c>
-      <c r="K9">
-        <v>17</v>
-      </c>
-      <c r="L9">
-        <v>12</v>
-      </c>
-      <c r="M9">
-        <v>3</v>
-      </c>
-      <c r="N9">
-        <v>4</v>
-      </c>
-      <c r="O9">
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10">
-        <v>-11</v>
-      </c>
-      <c r="E10">
-        <v>-9</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <v>12</v>
-      </c>
-      <c r="I10">
-        <v>17</v>
-      </c>
-      <c r="J10">
-        <v>17</v>
-      </c>
-      <c r="K10">
-        <v>18</v>
-      </c>
-      <c r="L10">
-        <v>10</v>
-      </c>
-      <c r="M10">
-        <v>2</v>
-      </c>
-      <c r="N10">
-        <v>3</v>
-      </c>
-      <c r="O10">
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11">
-        <v>-6</v>
-      </c>
-      <c r="E11">
-        <v>5</v>
-      </c>
-      <c r="F11">
-        <v>2</v>
-      </c>
-      <c r="G11">
-        <v>4</v>
-      </c>
-      <c r="H11">
-        <v>8</v>
-      </c>
-      <c r="I11">
-        <v>17</v>
-      </c>
-      <c r="J11">
-        <v>16</v>
-      </c>
-      <c r="K11">
-        <v>16</v>
-      </c>
-      <c r="L11">
-        <v>12</v>
-      </c>
-      <c r="M11">
-        <v>4</v>
-      </c>
-      <c r="N11">
-        <v>4</v>
-      </c>
-      <c r="O11">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12">
-        <v>-8</v>
-      </c>
-      <c r="E12">
-        <v>-11</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>6</v>
-      </c>
-      <c r="H12">
-        <v>7</v>
-      </c>
-      <c r="I12">
-        <v>15</v>
-      </c>
-      <c r="J12">
-        <v>17</v>
-      </c>
-      <c r="K12">
-        <v>17</v>
-      </c>
-      <c r="L12">
-        <v>11</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="N12">
-        <v>5</v>
-      </c>
-      <c r="O12">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13">
-        <v>-11</v>
-      </c>
-      <c r="E13">
-        <v>-12</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>7</v>
-      </c>
       <c r="H13">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I13">
         <v>14</v>
       </c>
       <c r="J13">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="K13">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="L13">
-        <v>11</v>
+        <v>-2</v>
       </c>
       <c r="M13">
-        <v>3</v>
-      </c>
-      <c r="N13">
-        <v>5</v>
-      </c>
-      <c r="O13">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>21</v>
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>-8</v>
+      </c>
+      <c r="C14">
+        <v>-5</v>
       </c>
       <c r="D14">
-        <v>-8</v>
+        <v>3</v>
       </c>
       <c r="E14">
-        <v>-9</v>
+        <v>8</v>
       </c>
       <c r="F14">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G14">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H14">
-        <v>5</v>
-      </c>
-      <c r="I14" t="s">
-        <v>55</v>
+        <v>16</v>
+      </c>
+      <c r="I14">
+        <v>15</v>
       </c>
       <c r="J14">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="K14">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="L14">
-        <v>12</v>
-      </c>
-      <c r="M14">
-        <v>4</v>
-      </c>
-      <c r="N14">
-        <v>-1</v>
-      </c>
-      <c r="O14">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15">
-        <v>-8</v>
-      </c>
-      <c r="E15">
-        <v>-6</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>8</v>
-      </c>
-      <c r="H15">
-        <v>5</v>
-      </c>
-      <c r="I15">
-        <v>14</v>
-      </c>
-      <c r="J15">
-        <v>15</v>
-      </c>
-      <c r="K15">
-        <v>14</v>
-      </c>
-      <c r="L15">
-        <v>10</v>
-      </c>
-      <c r="M15">
-        <v>2</v>
-      </c>
-      <c r="N15">
-        <v>-2</v>
-      </c>
-      <c r="O15">
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16">
-        <v>-8</v>
-      </c>
-      <c r="E16">
-        <v>-5</v>
-      </c>
-      <c r="F16">
-        <v>3</v>
-      </c>
-      <c r="G16">
-        <v>8</v>
-      </c>
-      <c r="H16">
-        <v>6</v>
-      </c>
-      <c r="I16">
-        <v>13</v>
-      </c>
-      <c r="J16">
-        <v>16</v>
-      </c>
-      <c r="K16">
-        <v>15</v>
-      </c>
-      <c r="L16">
-        <v>10</v>
-      </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
-      <c r="N16">
         <f>-1</f>
         <v>-1</v>
       </c>
-      <c r="O16">
+      <c r="M14">
         <v>-5</v>
       </c>
     </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
+      <c r="B15">
+        <v>-8</v>
+      </c>
+      <c r="C15">
+        <v>-4</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>9</v>
+      </c>
+      <c r="F15">
+        <v>8</v>
+      </c>
+      <c r="G15">
+        <v>11</v>
+      </c>
+      <c r="H15">
+        <v>16</v>
+      </c>
+      <c r="I15">
+        <v>15</v>
+      </c>
+      <c r="J15">
+        <v>9</v>
+      </c>
+      <c r="K15">
+        <v>3</v>
+      </c>
+      <c r="L15">
+        <v>-7</v>
+      </c>
+      <c r="M15">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>-10</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>10</v>
+      </c>
+      <c r="G16">
+        <v>14</v>
+      </c>
+      <c r="H16">
+        <v>13</v>
+      </c>
+      <c r="I16">
+        <v>15</v>
+      </c>
+      <c r="J16">
+        <v>9</v>
+      </c>
+      <c r="K16">
+        <v>3</v>
+      </c>
+      <c r="L16">
+        <v>-8</v>
+      </c>
+      <c r="M16">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>-10</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
       <c r="D17">
-        <v>-8</v>
+        <v>7</v>
       </c>
       <c r="E17">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>12</v>
+      </c>
+      <c r="G17">
+        <v>15</v>
+      </c>
+      <c r="H17">
+        <v>14</v>
+      </c>
+      <c r="I17">
+        <v>48</v>
+      </c>
+      <c r="J17">
+        <v>10</v>
+      </c>
+      <c r="K17">
+        <v>3</v>
+      </c>
+      <c r="L17">
+        <v>-5</v>
+      </c>
+      <c r="M17">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>-9</v>
+      </c>
+      <c r="C18">
+        <v>-9</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18">
+        <v>8</v>
+      </c>
+      <c r="F18">
+        <v>13</v>
+      </c>
+      <c r="G18">
+        <v>15</v>
+      </c>
+      <c r="H18">
+        <v>-6</v>
+      </c>
+      <c r="I18">
+        <v>18</v>
+      </c>
+      <c r="J18">
+        <v>11</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>-3</v>
+      </c>
+      <c r="M18">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <v>-6</v>
+      </c>
+      <c r="C19">
+        <v>-6</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>9</v>
+      </c>
+      <c r="F19">
+        <v>14</v>
+      </c>
+      <c r="G19">
+        <v>15</v>
+      </c>
+      <c r="H19">
+        <v>15</v>
+      </c>
+      <c r="I19">
+        <v>19</v>
+      </c>
+      <c r="J19">
+        <v>10</v>
+      </c>
+      <c r="K19">
+        <v>4</v>
+      </c>
+      <c r="L19">
+        <v>-2</v>
+      </c>
+      <c r="M19">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>-6</v>
+      </c>
+      <c r="C20">
+        <v>-6</v>
+      </c>
+      <c r="D20">
+        <v>-1</v>
+      </c>
+      <c r="E20">
+        <v>11</v>
+      </c>
+      <c r="F20">
+        <v>13</v>
+      </c>
+      <c r="G20">
+        <v>17</v>
+      </c>
+      <c r="H20">
+        <v>15</v>
+      </c>
+      <c r="I20">
+        <v>21</v>
+      </c>
+      <c r="J20">
+        <v>10</v>
+      </c>
+      <c r="K20">
+        <v>6</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
         <v>-4</v>
       </c>
-      <c r="F17">
-        <v>5</v>
-      </c>
-      <c r="G17">
+      <c r="C21">
+        <v>-4</v>
+      </c>
+      <c r="D21">
+        <v>-2</v>
+      </c>
+      <c r="E21">
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>15</v>
+      </c>
+      <c r="G21">
+        <v>16</v>
+      </c>
+      <c r="H21">
+        <v>15</v>
+      </c>
+      <c r="I21">
+        <v>24</v>
+      </c>
+      <c r="J21">
         <v>9</v>
       </c>
-      <c r="H17">
-        <v>8</v>
-      </c>
-      <c r="I17">
-        <v>11</v>
-      </c>
-      <c r="J17">
-        <v>16</v>
-      </c>
-      <c r="K17">
-        <v>15</v>
-      </c>
-      <c r="L17">
-        <v>9</v>
-      </c>
-      <c r="M17">
-        <v>3</v>
-      </c>
-      <c r="N17">
-        <v>-7</v>
-      </c>
-      <c r="O17">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18">
-        <v>-10</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>5</v>
-      </c>
-      <c r="G18">
-        <v>10</v>
-      </c>
-      <c r="H18">
-        <v>10</v>
-      </c>
-      <c r="I18">
-        <v>14</v>
-      </c>
-      <c r="J18">
-        <v>13</v>
-      </c>
-      <c r="K18">
-        <v>15</v>
-      </c>
-      <c r="L18">
-        <v>9</v>
-      </c>
-      <c r="M18">
-        <v>3</v>
-      </c>
-      <c r="N18">
-        <v>-8</v>
-      </c>
-      <c r="O18">
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19">
-        <v>-10</v>
-      </c>
-      <c r="E19">
-        <v>3</v>
-      </c>
-      <c r="F19">
-        <v>7</v>
-      </c>
-      <c r="G19">
-        <v>8</v>
-      </c>
-      <c r="H19">
-        <v>12</v>
-      </c>
-      <c r="I19">
-        <v>15</v>
-      </c>
-      <c r="J19">
-        <v>14</v>
-      </c>
-      <c r="K19">
-        <v>48</v>
-      </c>
-      <c r="L19">
-        <v>10</v>
-      </c>
-      <c r="M19">
-        <v>3</v>
-      </c>
-      <c r="N19">
-        <v>-5</v>
-      </c>
-      <c r="O19">
-        <v>-11</v>
-      </c>
-    </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20">
-        <v>-9</v>
-      </c>
-      <c r="E20">
-        <v>-9</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20">
-        <v>8</v>
-      </c>
-      <c r="H20">
-        <v>13</v>
-      </c>
-      <c r="I20">
-        <v>15</v>
-      </c>
-      <c r="J20">
-        <v>-6</v>
-      </c>
-      <c r="K20">
-        <v>18</v>
-      </c>
-      <c r="L20">
-        <v>11</v>
-      </c>
-      <c r="M20">
-        <v>1</v>
-      </c>
-      <c r="N20">
-        <v>-3</v>
-      </c>
-      <c r="O20">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21">
-        <v>-6</v>
-      </c>
-      <c r="E21">
-        <v>-6</v>
-      </c>
-      <c r="F21">
+      <c r="K21">
+        <v>6</v>
+      </c>
+      <c r="L21">
         <v>2</v>
       </c>
-      <c r="G21">
-        <v>9</v>
-      </c>
-      <c r="H21">
-        <v>14</v>
-      </c>
-      <c r="I21">
-        <v>15</v>
-      </c>
-      <c r="J21">
-        <v>15</v>
-      </c>
-      <c r="K21">
-        <v>19</v>
-      </c>
-      <c r="L21">
-        <v>10</v>
-      </c>
       <c r="M21">
-        <v>4</v>
-      </c>
-      <c r="N21">
-        <v>-2</v>
-      </c>
-      <c r="O21">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>29</v>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22">
+        <v>-8</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
       </c>
       <c r="D22">
-        <v>-6</v>
-      </c>
-      <c r="E22">
-        <v>-6</v>
-      </c>
-      <c r="F22">
-        <v>-1</v>
-      </c>
-      <c r="G22">
-        <v>11</v>
-      </c>
-      <c r="H22">
-        <v>13</v>
-      </c>
-      <c r="I22">
-        <v>17</v>
-      </c>
-      <c r="J22">
-        <v>15</v>
-      </c>
-      <c r="K22">
-        <v>21</v>
-      </c>
-      <c r="L22">
-        <v>10</v>
-      </c>
-      <c r="M22">
-        <v>6</v>
-      </c>
-      <c r="N22">
-        <v>1</v>
-      </c>
-      <c r="O22">
-        <v>-11</v>
-      </c>
-    </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23">
-        <v>-4</v>
-      </c>
-      <c r="E23">
-        <v>-4</v>
-      </c>
-      <c r="F23">
-        <v>-2</v>
-      </c>
-      <c r="G23">
-        <v>10</v>
-      </c>
-      <c r="H23">
-        <v>15</v>
-      </c>
-      <c r="I23">
-        <v>16</v>
-      </c>
-      <c r="J23">
-        <v>15</v>
-      </c>
-      <c r="K23">
-        <v>24</v>
-      </c>
-      <c r="L23">
-        <v>9</v>
-      </c>
-      <c r="M23">
-        <v>6</v>
-      </c>
-      <c r="N23">
-        <v>2</v>
-      </c>
-      <c r="O23">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24">
-        <v>-8</v>
-      </c>
-      <c r="E24">
-        <v>2</v>
-      </c>
-      <c r="F24">
         <f>-1</f>
         <v>-1</v>
       </c>
+      <c r="E22">
+        <v>11</v>
+      </c>
+      <c r="F22">
+        <v>15</v>
+      </c>
+      <c r="G22">
+        <v>19</v>
+      </c>
+      <c r="H22">
+        <v>17</v>
+      </c>
+      <c r="I22">
+        <v>21</v>
+      </c>
+      <c r="J22">
+        <v>11</v>
+      </c>
+      <c r="K22">
+        <v>6</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>-9</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>12</v>
+      </c>
+      <c r="F23">
+        <v>15</v>
+      </c>
+      <c r="G23">
+        <v>20</v>
+      </c>
+      <c r="H23">
+        <v>18</v>
+      </c>
+      <c r="I23">
+        <v>21</v>
+      </c>
+      <c r="J23">
+        <v>12</v>
+      </c>
+      <c r="K23">
+        <v>7</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>-33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24">
+        <v>-14</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>9</v>
+      </c>
+      <c r="F24">
+        <v>18</v>
+      </c>
       <c r="G24">
+        <v>19</v>
+      </c>
+      <c r="H24">
+        <v>19</v>
+      </c>
+      <c r="I24">
+        <v>26</v>
+      </c>
+      <c r="J24">
+        <v>12</v>
+      </c>
+      <c r="K24">
+        <v>7</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25">
+        <v>-15</v>
+      </c>
+      <c r="C25">
+        <v>-3</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>18</v>
+      </c>
+      <c r="G25">
+        <v>20</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I25">
+        <v>17</v>
+      </c>
+      <c r="J25">
+        <v>10</v>
+      </c>
+      <c r="K25">
+        <v>6</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26">
+        <v>-17</v>
+      </c>
+      <c r="C26">
+        <v>-4</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>8</v>
+      </c>
+      <c r="F26">
+        <v>16</v>
+      </c>
+      <c r="G26">
+        <v>22</v>
+      </c>
+      <c r="H26">
+        <v>24</v>
+      </c>
+      <c r="I26">
+        <v>18</v>
+      </c>
+      <c r="J26">
         <v>11</v>
       </c>
-      <c r="H24">
-        <v>15</v>
-      </c>
-      <c r="I24">
-        <v>19</v>
-      </c>
-      <c r="J24">
-        <v>17</v>
-      </c>
-      <c r="K24">
+      <c r="K26">
+        <v>6</v>
+      </c>
+      <c r="L26">
+        <v>3</v>
+      </c>
+      <c r="M26">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27">
+        <v>-19</v>
+      </c>
+      <c r="C27">
+        <v>-6</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>8</v>
+      </c>
+      <c r="F27">
+        <v>15</v>
+      </c>
+      <c r="G27">
+        <v>22</v>
+      </c>
+      <c r="H27">
+        <v>23</v>
+      </c>
+      <c r="I27">
+        <v>17</v>
+      </c>
+      <c r="J27">
+        <v>10</v>
+      </c>
+      <c r="K27">
+        <v>6</v>
+      </c>
+      <c r="L27">
+        <v>5</v>
+      </c>
+      <c r="M27">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28">
+        <v>-23</v>
+      </c>
+      <c r="C28">
+        <v>-8</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>6</v>
+      </c>
+      <c r="F28">
+        <v>16</v>
+      </c>
+      <c r="G28">
         <v>21</v>
       </c>
-      <c r="L24">
+      <c r="H28">
+        <v>26</v>
+      </c>
+      <c r="I28">
+        <v>17</v>
+      </c>
+      <c r="J28">
+        <v>9</v>
+      </c>
+      <c r="K28">
+        <v>4</v>
+      </c>
+      <c r="L28">
+        <v>-2</v>
+      </c>
+      <c r="M28">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29">
+        <v>-8</v>
+      </c>
+      <c r="C29">
+        <v>-8</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <v>9</v>
+      </c>
+      <c r="F29">
+        <v>16</v>
+      </c>
+      <c r="G29">
+        <v>22</v>
+      </c>
+      <c r="H29">
+        <v>26</v>
+      </c>
+      <c r="I29">
+        <v>16</v>
+      </c>
+      <c r="J29">
+        <v>6</v>
+      </c>
+      <c r="K29">
+        <v>3</v>
+      </c>
+      <c r="L29">
+        <v>-3</v>
+      </c>
+      <c r="M29">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30">
+        <v>-9</v>
+      </c>
+      <c r="C30">
+        <v>-11</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+      <c r="E30">
         <v>11</v>
       </c>
-      <c r="M24">
+      <c r="F30">
+        <v>17</v>
+      </c>
+      <c r="G30">
+        <v>21</v>
+      </c>
+      <c r="H30">
+        <v>21</v>
+      </c>
+      <c r="I30">
+        <v>17</v>
+      </c>
+      <c r="J30">
+        <v>7</v>
+      </c>
+      <c r="K30">
+        <v>3</v>
+      </c>
+      <c r="L30">
+        <v>-6</v>
+      </c>
+      <c r="M30">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <v>-5</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>14</v>
+      </c>
+      <c r="F31">
+        <v>16</v>
+      </c>
+      <c r="G31">
+        <v>21</v>
+      </c>
+      <c r="H31">
+        <v>22</v>
+      </c>
+      <c r="I31">
+        <v>17</v>
+      </c>
+      <c r="J31">
+        <v>7</v>
+      </c>
+      <c r="K31">
+        <v>4</v>
+      </c>
+      <c r="L31">
+        <v>-6</v>
+      </c>
+      <c r="M31">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32">
+        <v>-6</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <v>16</v>
+      </c>
+      <c r="F32">
+        <v>17</v>
+      </c>
+      <c r="G32">
+        <v>17</v>
+      </c>
+      <c r="H32">
+        <v>23</v>
+      </c>
+      <c r="I32">
+        <v>18</v>
+      </c>
+      <c r="J32">
         <v>6</v>
       </c>
-      <c r="N24">
-        <v>1</v>
-      </c>
-      <c r="O24">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25">
-        <v>-9</v>
-      </c>
-      <c r="E25">
-        <v>3</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>12</v>
-      </c>
-      <c r="H25">
-        <v>15</v>
-      </c>
-      <c r="I25">
-        <v>20</v>
-      </c>
-      <c r="J25">
-        <v>18</v>
-      </c>
-      <c r="K25">
-        <v>21</v>
-      </c>
-      <c r="L25">
-        <v>12</v>
-      </c>
-      <c r="M25">
-        <v>7</v>
-      </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="O25">
-        <v>-33</v>
-      </c>
-    </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26">
-        <v>-14</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>9</v>
-      </c>
-      <c r="H26">
-        <v>18</v>
-      </c>
-      <c r="I26">
-        <v>19</v>
-      </c>
-      <c r="J26">
-        <v>19</v>
-      </c>
-      <c r="K26">
-        <v>26</v>
-      </c>
-      <c r="L26">
-        <v>12</v>
-      </c>
-      <c r="M26">
-        <v>7</v>
-      </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-      <c r="O26">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27">
-        <v>-15</v>
-      </c>
-      <c r="E27">
-        <v>-3</v>
-      </c>
-      <c r="F27">
+      <c r="K32">
         <v>2</v>
       </c>
-      <c r="G27">
-        <v>7</v>
-      </c>
-      <c r="H27">
-        <v>18</v>
-      </c>
-      <c r="I27">
-        <v>20</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K27">
-        <v>17</v>
-      </c>
-      <c r="L27">
-        <v>10</v>
-      </c>
-      <c r="M27">
-        <v>6</v>
-      </c>
-      <c r="N27">
-        <v>1</v>
-      </c>
-      <c r="O27">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28">
-        <v>-17</v>
-      </c>
-      <c r="E28">
+      <c r="L32">
         <v>-4</v>
       </c>
-      <c r="F28">
-        <v>3</v>
-      </c>
-      <c r="G28">
-        <v>8</v>
-      </c>
-      <c r="H28">
-        <v>16</v>
-      </c>
-      <c r="I28">
-        <v>22</v>
-      </c>
-      <c r="J28">
-        <v>24</v>
-      </c>
-      <c r="K28">
-        <v>18</v>
-      </c>
-      <c r="L28">
-        <v>11</v>
-      </c>
-      <c r="M28">
-        <v>6</v>
-      </c>
-      <c r="N28">
-        <v>3</v>
-      </c>
-      <c r="O28">
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29">
-        <v>-19</v>
-      </c>
-      <c r="E29">
-        <v>-6</v>
-      </c>
-      <c r="F29">
-        <v>4</v>
-      </c>
-      <c r="G29">
-        <v>8</v>
-      </c>
-      <c r="H29">
-        <v>15</v>
-      </c>
-      <c r="I29">
-        <v>22</v>
-      </c>
-      <c r="J29">
-        <v>23</v>
-      </c>
-      <c r="K29">
-        <v>17</v>
-      </c>
-      <c r="L29">
-        <v>10</v>
-      </c>
-      <c r="M29">
-        <v>6</v>
-      </c>
-      <c r="N29">
-        <v>5</v>
-      </c>
-      <c r="O29">
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30">
-        <v>-23</v>
-      </c>
-      <c r="E30">
-        <v>-8</v>
-      </c>
-      <c r="F30">
-        <v>3</v>
-      </c>
-      <c r="G30">
-        <v>6</v>
-      </c>
-      <c r="H30">
-        <v>16</v>
-      </c>
-      <c r="I30">
-        <v>21</v>
-      </c>
-      <c r="J30">
-        <v>26</v>
-      </c>
-      <c r="K30">
-        <v>17</v>
-      </c>
-      <c r="L30">
-        <v>9</v>
-      </c>
-      <c r="M30">
-        <v>4</v>
-      </c>
-      <c r="N30">
-        <v>-2</v>
-      </c>
-      <c r="O30">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31">
-        <v>-8</v>
-      </c>
-      <c r="E31">
-        <v>-8</v>
-      </c>
-      <c r="F31">
-        <v>4</v>
-      </c>
-      <c r="G31">
-        <v>9</v>
-      </c>
-      <c r="H31">
-        <v>16</v>
-      </c>
-      <c r="I31">
-        <v>22</v>
-      </c>
-      <c r="J31">
-        <v>26</v>
-      </c>
-      <c r="K31">
-        <v>16</v>
-      </c>
-      <c r="L31">
-        <v>6</v>
-      </c>
-      <c r="M31">
-        <v>3</v>
-      </c>
-      <c r="N31">
-        <v>-3</v>
-      </c>
-      <c r="O31">
+      <c r="M32">
         <v>-7</v>
       </c>
     </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32">
-        <v>-9</v>
-      </c>
-      <c r="E32">
-        <v>-11</v>
-      </c>
-      <c r="F32">
-        <v>5</v>
-      </c>
-      <c r="G32">
-        <v>11</v>
-      </c>
-      <c r="H32">
-        <v>17</v>
-      </c>
-      <c r="I32">
-        <v>21</v>
-      </c>
-      <c r="J32">
-        <v>21</v>
-      </c>
-      <c r="K32">
-        <v>17</v>
-      </c>
-      <c r="L32">
-        <v>7</v>
-      </c>
-      <c r="M32">
-        <v>3</v>
-      </c>
-      <c r="N32">
-        <v>-6</v>
-      </c>
-      <c r="O32">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>40</v>
-      </c>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33">
+        <v>-7</v>
+      </c>
+      <c r="C33" s="1"/>
       <c r="D33">
-        <v>-5</v>
+        <v>3</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33">
-        <v>5</v>
-      </c>
-      <c r="G33">
-        <v>14</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="G33" s="1"/>
       <c r="H33">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I33">
-        <v>21</v>
-      </c>
-      <c r="J33">
-        <v>22</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="J33" s="1"/>
       <c r="K33">
-        <v>17</v>
-      </c>
-      <c r="L33">
-        <v>7</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="L33" s="1"/>
       <c r="M33">
-        <v>4</v>
-      </c>
-      <c r="N33">
-        <v>-6</v>
-      </c>
-      <c r="O33">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>41</v>
-      </c>
-      <c r="D34">
-        <v>-6</v>
-      </c>
-      <c r="E34" s="1"/>
-      <c r="F34">
-        <v>3</v>
-      </c>
-      <c r="G34">
-        <v>16</v>
-      </c>
-      <c r="H34">
-        <v>17</v>
-      </c>
-      <c r="I34">
-        <v>17</v>
-      </c>
-      <c r="J34">
-        <v>23</v>
-      </c>
-      <c r="K34">
-        <v>18</v>
-      </c>
-      <c r="L34">
-        <v>6</v>
-      </c>
-      <c r="M34">
-        <v>2</v>
-      </c>
-      <c r="N34">
-        <v>-4</v>
-      </c>
-      <c r="O34">
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>42</v>
-      </c>
-      <c r="D35">
-        <v>-7</v>
-      </c>
-      <c r="E35" s="1"/>
-      <c r="F35">
-        <v>3</v>
-      </c>
-      <c r="G35" s="1"/>
-      <c r="H35">
-        <v>17</v>
-      </c>
-      <c r="I35" s="1"/>
-      <c r="J35">
-        <v>21</v>
-      </c>
-      <c r="K35">
-        <v>17</v>
-      </c>
-      <c r="L35" s="1"/>
-      <c r="M35">
-        <v>1</v>
-      </c>
-      <c r="N35" s="1"/>
-      <c r="O35">
         <v>-5</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B41" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" t="s">
         <v>51</v>
       </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D43" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>46</v>
-      </c>
-      <c r="D44" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>44</v>
-      </c>
-      <c r="D45" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Script de traitement de la feuille erreurs
</commit_message>
<xml_diff>
--- a/graph/Climat.xlsx
+++ b/graph/Climat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bivaudb/Desktop/EPSI/QUALITE DES DONNES/TP1_Qualite_Donnees/graph/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8DC62D-700F-8649-82FF-054AC9A81D82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82785474-EC35-8B45-A5E6-5686D05718E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="45">
   <si>
     <t>janvier</t>
   </si>
@@ -166,55 +166,10 @@
     <t>J31</t>
   </si>
   <si>
-    <t>moyenne</t>
-  </si>
-  <si>
-    <t>écart type</t>
-  </si>
-  <si>
-    <t>min /max</t>
-  </si>
-  <si>
     <t>0xFFFF</t>
   </si>
   <si>
-    <t>identifier les valeurs atypiques ou manquantes</t>
-  </si>
-  <si>
-    <t>définir une méthode pour identifier une valeur atypique</t>
-  </si>
-  <si>
-    <t>pour cet échantillon :</t>
-  </si>
-  <si>
-    <t>calculer</t>
-  </si>
-  <si>
-    <t>par mois</t>
-  </si>
-  <si>
-    <t>par mois et par année</t>
-  </si>
-  <si>
-    <t>présenter la valeur lue en parcourant la courbe à l'aide du pointeur, présenter les valeurs précédentes par mois et par année, par mois glissant de 30 jours centré sur la valeur lue</t>
-  </si>
-  <si>
     <t>Sun</t>
-  </si>
-  <si>
-    <t>tracer les coubes de chaque mois avec une bibliothèque grapohique python</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assembler les courbes sur un seul graphique (J1 -&gt; J365) </t>
-  </si>
-  <si>
-    <t>utiliser par exemple  Python Scipy pour les parties mathématiques</t>
-  </si>
-  <si>
-    <t>définir une loi pour valider la pertinence ou non d'une valeur atypique</t>
-  </si>
-  <si>
-    <t>implémenter ces lois dans votre application précédente</t>
   </si>
 </sst>
 </file>
@@ -2079,10 +2034,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2444,7 +2399,7 @@
         <v>11</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L9">
         <v>5</v>
@@ -2514,7 +2469,7 @@
         <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="H11">
         <v>15</v>
@@ -2752,7 +2707,7 @@
         <v>-9</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E17">
         <v>8</v>
@@ -3052,7 +3007,7 @@
         <v>20</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I24">
         <v>17</v>
@@ -3382,78 +3337,6 @@
       <c r="L32" s="1"/>
       <c r="M32">
         <v>-5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>45</v>
-      </c>
-      <c r="D41" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>44</v>
-      </c>
-      <c r="D42" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>